<commit_message>
added model design for weather
</commit_message>
<xml_diff>
--- a/files/Client_Cash_Accounts.xlsx
+++ b/files/Client_Cash_Accounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophershi/Dev/fins3645/assignment/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B2DA4C-33CA-EB4B-A668-9420F318D539}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8410ABAA-569D-184A-AD27-E5467CBAB375}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="460" windowWidth="26000" windowHeight="18620" activeTab="3" xr2:uid="{1E40420A-6C34-45C8-A5DC-E0E21BBDF318}"/>
+    <workbookView xWindow="3000" yWindow="460" windowWidth="26000" windowHeight="18620" xr2:uid="{1E40420A-6C34-45C8-A5DC-E0E21BBDF318}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -1001,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A59172-0B3A-41DF-B82B-3691A47F5C10}">
   <dimension ref="A1:H210"/>
   <sheetViews>
-    <sheetView topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="I20" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7704,7 +7704,7 @@
   <dimension ref="A1:C123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16618,7 +16618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F87782D-9858-4DF3-B128-50991DBD144F}">
   <dimension ref="A1:C123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>